<commit_message>
Fixed some sychronization issues.
</commit_message>
<xml_diff>
--- a/src/test/resources/TAS-2_Employee_data.xlsx
+++ b/src/test/resources/TAS-2_Employee_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
   <si>
     <t>Firstname*</t>
   </si>
@@ -272,6 +272,63 @@
   <si>
     <t>5 Year</t>
   </si>
+  <si>
+    <t>3 Year</t>
+  </si>
+  <si>
+    <t>0 month</t>
+  </si>
+  <si>
+    <t>15 Days</t>
+  </si>
+  <si>
+    <t>4 Year</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>16 Days</t>
+  </si>
+  <si>
+    <t>2 month</t>
+  </si>
+  <si>
+    <t>17 Days</t>
+  </si>
+  <si>
+    <t>6 Year</t>
+  </si>
+  <si>
+    <t>3 month</t>
+  </si>
+  <si>
+    <t>18 Days</t>
+  </si>
+  <si>
+    <t>Arshad</t>
+  </si>
+  <si>
+    <t>Bikash</t>
+  </si>
+  <si>
+    <t>Abhi</t>
+  </si>
+  <si>
+    <t>Niki</t>
+  </si>
+  <si>
+    <t>ar124@gmail.com</t>
+  </si>
+  <si>
+    <t>bk124@gmail.com</t>
+  </si>
+  <si>
+    <t>ab124@gmail.com</t>
+  </si>
+  <si>
+    <t>nk124@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -281,12 +338,19 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -354,58 +418,60 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1121,15 +1187,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1191,9 +1258,129 @@
         <v>78</v>
       </c>
     </row>
+    <row r="3" spans="1:9" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7008955489</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7008955490</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7008955491</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7008955492</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added fix to OnBoardingPage.
</commit_message>
<xml_diff>
--- a/src/test/resources/TAS-2_Employee_data.xlsx
+++ b/src/test/resources/TAS-2_Employee_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
   <si>
     <t>Firstname*</t>
   </si>
@@ -282,52 +282,10 @@
     <t>15 Days</t>
   </si>
   <si>
-    <t>4 Year</t>
-  </si>
-  <si>
-    <t>1 month</t>
-  </si>
-  <si>
-    <t>16 Days</t>
-  </si>
-  <si>
-    <t>2 month</t>
-  </si>
-  <si>
-    <t>17 Days</t>
-  </si>
-  <si>
-    <t>6 Year</t>
-  </si>
-  <si>
-    <t>3 month</t>
-  </si>
-  <si>
-    <t>18 Days</t>
-  </si>
-  <si>
     <t>Arshad</t>
   </si>
   <si>
-    <t>Bikash</t>
-  </si>
-  <si>
-    <t>Abhi</t>
-  </si>
-  <si>
-    <t>Niki</t>
-  </si>
-  <si>
     <t>ar124@gmail.com</t>
-  </si>
-  <si>
-    <t>bk124@gmail.com</t>
-  </si>
-  <si>
-    <t>ab124@gmail.com</t>
-  </si>
-  <si>
-    <t>nk124@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1187,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1260,10 +1218,10 @@
     </row>
     <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1">
         <v>7008955489</v>
@@ -1285,102 +1243,12 @@
       </c>
       <c r="I3" s="23" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7008955490</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3.12</v>
-      </c>
-      <c r="H4" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7008955491</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="H5" s="1">
-        <v>5.9</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7008955492</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5.3</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Changes merged from latest change from master
</commit_message>
<xml_diff>
--- a/src/test/resources/TAS-2_Employee_data.xlsx
+++ b/src/test/resources/TAS-2_Employee_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>Firstname*</t>
   </si>
@@ -256,23 +256,9 @@
     <t>QA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>30 Days</t>
-    </r>
-  </si>
-  <si>
     <t>5 month</t>
   </si>
   <si>
-    <t>5 Year</t>
-  </si>
-  <si>
     <t>3 Year</t>
   </si>
   <si>
@@ -286,6 +272,105 @@
   </si>
   <si>
     <t>ar124@gmail.com</t>
+  </si>
+  <si>
+    <t>Subha</t>
+  </si>
+  <si>
+    <t>sb11@gmail.com</t>
+  </si>
+  <si>
+    <t>4 Year</t>
+  </si>
+  <si>
+    <t>Abhi</t>
+  </si>
+  <si>
+    <t>ab11@gmail.com</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>2 month</t>
+  </si>
+  <si>
+    <t>Niki</t>
+  </si>
+  <si>
+    <t>6 Year</t>
+  </si>
+  <si>
+    <t>3 month</t>
+  </si>
+  <si>
+    <t>7 Year</t>
+  </si>
+  <si>
+    <t>4 month</t>
+  </si>
+  <si>
+    <t>8 Year</t>
+  </si>
+  <si>
+    <t>9 Year</t>
+  </si>
+  <si>
+    <t>6 month</t>
+  </si>
+  <si>
+    <t>10 Year</t>
+  </si>
+  <si>
+    <t>7 month</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Shiv</t>
+  </si>
+  <si>
+    <t>Arman</t>
+  </si>
+  <si>
+    <t>aks</t>
+  </si>
+  <si>
+    <t>45 Days</t>
+  </si>
+  <si>
+    <t>90 Days</t>
+  </si>
+  <si>
+    <t>60 Days</t>
+  </si>
+  <si>
+    <t>gnk22@gmail.com</t>
+  </si>
+  <si>
+    <t>ynk22@gmail.com</t>
+  </si>
+  <si>
+    <t>unk22@gmail.com</t>
+  </si>
+  <si>
+    <t>yynk22@gmail.com</t>
+  </si>
+  <si>
+    <t>oonk22@gmail.com</t>
+  </si>
+  <si>
+    <t>oks</t>
+  </si>
+  <si>
+    <t>pks22@gmail.com</t>
+  </si>
+  <si>
+    <t>30 Days</t>
+  </si>
+  <si>
+    <t>2 Year</t>
   </si>
 </sst>
 </file>
@@ -296,12 +381,26 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -376,59 +475,61 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1145,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1201,10 +1302,10 @@
         <v>77</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="1">
         <v>5</v>
@@ -1213,15 +1314,15 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1">
         <v>7008955489</v>
@@ -1230,10 +1331,10 @@
         <v>77</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G3" s="1">
         <v>2.62</v>
@@ -1242,13 +1343,253 @@
         <v>5.6</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>7008957789</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2378654879</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2378654880</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2378654881</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H7" s="1">
+        <v>9</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
+      <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2378654882</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
+      <c r="A9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2378654883</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
+      <c r="A10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2378654884</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H10" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
+      <c r="A11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2378634884</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added new emp data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TAS-2_Employee_data.xlsx
+++ b/src/test/resources/TAS-2_Employee_data.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="empSheet" sheetId="1" r:id="rId1"/>
     <sheet name="OnBoardData" sheetId="2" r:id="rId2"/>
+    <sheet name="delEmpData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="318">
   <si>
     <t>Firstname*</t>
   </si>
@@ -247,12 +248,6 @@
     <t>NpDay</t>
   </si>
   <si>
-    <t>Dipak</t>
-  </si>
-  <si>
-    <t>db123@gmail.com</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -268,36 +263,15 @@
     <t>15 Days</t>
   </si>
   <si>
-    <t>Arshad</t>
-  </si>
-  <si>
-    <t>ar124@gmail.com</t>
-  </si>
-  <si>
-    <t>Subha</t>
-  </si>
-  <si>
-    <t>sb11@gmail.com</t>
-  </si>
-  <si>
     <t>4 Year</t>
   </si>
   <si>
-    <t>Abhi</t>
-  </si>
-  <si>
-    <t>ab11@gmail.com</t>
-  </si>
-  <si>
     <t>1 month</t>
   </si>
   <si>
     <t>2 month</t>
   </si>
   <si>
-    <t>Niki</t>
-  </si>
-  <si>
     <t>6 Year</t>
   </si>
   <si>
@@ -325,18 +299,6 @@
     <t>7 month</t>
   </si>
   <si>
-    <t>Ramesh</t>
-  </si>
-  <si>
-    <t>Shiv</t>
-  </si>
-  <si>
-    <t>Arman</t>
-  </si>
-  <si>
-    <t>aks</t>
-  </si>
-  <si>
     <t>45 Days</t>
   </si>
   <si>
@@ -346,31 +308,673 @@
     <t>60 Days</t>
   </si>
   <si>
-    <t>gnk22@gmail.com</t>
-  </si>
-  <si>
-    <t>ynk22@gmail.com</t>
-  </si>
-  <si>
-    <t>unk22@gmail.com</t>
-  </si>
-  <si>
-    <t>yynk22@gmail.com</t>
-  </si>
-  <si>
-    <t>oonk22@gmail.com</t>
-  </si>
-  <si>
-    <t>oks</t>
-  </si>
-  <si>
-    <t>pks22@gmail.com</t>
-  </si>
-  <si>
     <t>30 Days</t>
   </si>
   <si>
     <t>2 Year</t>
+  </si>
+  <si>
+    <t>wmante@yahoo.com</t>
+  </si>
+  <si>
+    <t>carolyne.wolf@glover.com</t>
+  </si>
+  <si>
+    <t>istoltenberg@gmail.com</t>
+  </si>
+  <si>
+    <t>taya13@reilly.com</t>
+  </si>
+  <si>
+    <t>effertz.john@casper.com</t>
+  </si>
+  <si>
+    <t>jonas94@yahoo.com</t>
+  </si>
+  <si>
+    <t>ankunding.bryce@hotmail.com</t>
+  </si>
+  <si>
+    <t>elwyn.mayer@runte.com</t>
+  </si>
+  <si>
+    <t>ischowalter@yahoo.com</t>
+  </si>
+  <si>
+    <t>kennedi.ohara@morar.net</t>
+  </si>
+  <si>
+    <t>bo.wehner@gmail.com</t>
+  </si>
+  <si>
+    <t>feil.kenna@gmail.com</t>
+  </si>
+  <si>
+    <t>horn@gmail.com</t>
+  </si>
+  <si>
+    <t>darien76@gaylord.net</t>
+  </si>
+  <si>
+    <t>hailey.stiedemann@gmail.com</t>
+  </si>
+  <si>
+    <t>kunde.river@mayert.com</t>
+  </si>
+  <si>
+    <t>lang.eda@hotmail.com</t>
+  </si>
+  <si>
+    <t>henriette.thiel@hotmail.com</t>
+  </si>
+  <si>
+    <t>jaskolski.frederic@yahoo.com</t>
+  </si>
+  <si>
+    <t>lockman.boyd@gorczany.info</t>
+  </si>
+  <si>
+    <t>sanford.veda@yahoo.com</t>
+  </si>
+  <si>
+    <t>dmaggio@rath.com</t>
+  </si>
+  <si>
+    <t>bergnaum.dino@jaskolski.com</t>
+  </si>
+  <si>
+    <t>gernser@hotmail.com</t>
+  </si>
+  <si>
+    <t>harvey.cletus@gmail.com</t>
+  </si>
+  <si>
+    <t>clara.keebler@hotmail.com</t>
+  </si>
+  <si>
+    <t>uhilpert@yahoo.com</t>
+  </si>
+  <si>
+    <t>clair05@lubowitz.com</t>
+  </si>
+  <si>
+    <t>lgutmann@corwin.net</t>
+  </si>
+  <si>
+    <t>idickens@lakin.com</t>
+  </si>
+  <si>
+    <t>tate31@hotmail.com</t>
+  </si>
+  <si>
+    <t>parker.jovan@yahoo.com</t>
+  </si>
+  <si>
+    <t>khammes@walsh.com</t>
+  </si>
+  <si>
+    <t>kessler.linda@willms.com</t>
+  </si>
+  <si>
+    <t>demond17@hotmail.com</t>
+  </si>
+  <si>
+    <t>gbechtelar@yahoo.com</t>
+  </si>
+  <si>
+    <t>elouise99@cummings.info</t>
+  </si>
+  <si>
+    <t>ireichert@hotmail.com</t>
+  </si>
+  <si>
+    <t>weimann.larue@johnston.org</t>
+  </si>
+  <si>
+    <t>vnader@volkman.biz</t>
+  </si>
+  <si>
+    <t>ucrist@dubuque.com</t>
+  </si>
+  <si>
+    <t>arvel.ernser@gmail.com</t>
+  </si>
+  <si>
+    <t>stamm.ashley@marks.net</t>
+  </si>
+  <si>
+    <t>arvilla02@zboncak.biz</t>
+  </si>
+  <si>
+    <t>keeling.sheldon@yahoo.com</t>
+  </si>
+  <si>
+    <t>weissnat.eva@yahoo.com</t>
+  </si>
+  <si>
+    <t>krystal.gorczany@pollich.com</t>
+  </si>
+  <si>
+    <t>efren58@kulas.com</t>
+  </si>
+  <si>
+    <t>franz38@homenick.org</t>
+  </si>
+  <si>
+    <t>goodwin.isadore@yahoo.com</t>
+  </si>
+  <si>
+    <t>ppaucek@gmail.com</t>
+  </si>
+  <si>
+    <t>thurman.kohler@hotmail.com</t>
+  </si>
+  <si>
+    <t>laverna49@runolfsdottir.com</t>
+  </si>
+  <si>
+    <t>hartmann.vickie@gmail.com</t>
+  </si>
+  <si>
+    <t>gerhold.audie@gmail.com</t>
+  </si>
+  <si>
+    <t>ohyatt@bosco.biz</t>
+  </si>
+  <si>
+    <t>vandervort.josiane@hotmail.com</t>
+  </si>
+  <si>
+    <t>jgottlieb@hotmail.com</t>
+  </si>
+  <si>
+    <t>schultz.gay@metz.com</t>
+  </si>
+  <si>
+    <t>wiza.dane@gmail.com</t>
+  </si>
+  <si>
+    <t>vilma.larkin@dooley.com</t>
+  </si>
+  <si>
+    <t>estelle.schaefer@yahoo.com</t>
+  </si>
+  <si>
+    <t>emmitt.crooks@senger.info</t>
+  </si>
+  <si>
+    <t>dell98@bernhard.com</t>
+  </si>
+  <si>
+    <t>preinger@gmail.com</t>
+  </si>
+  <si>
+    <t>casper.ludie@fahey.com</t>
+  </si>
+  <si>
+    <t>leo60@goldner.net</t>
+  </si>
+  <si>
+    <t>helga.schroeder@stehr.com</t>
+  </si>
+  <si>
+    <t>carroll.yesenia@greenholt.com</t>
+  </si>
+  <si>
+    <t>laurine.senger@hotmail.com</t>
+  </si>
+  <si>
+    <t>buddy.jenkins@mann.com</t>
+  </si>
+  <si>
+    <t>grace.conroy@adams.com</t>
+  </si>
+  <si>
+    <t>vgerhold@hamill.com</t>
+  </si>
+  <si>
+    <t>qkuphal@gulgowski.biz</t>
+  </si>
+  <si>
+    <t>rowland84@yundt.com</t>
+  </si>
+  <si>
+    <t>quincy09@rath.com</t>
+  </si>
+  <si>
+    <t>stanford.pfannerstill@mann.com</t>
+  </si>
+  <si>
+    <t>vondricka@hotmail.com</t>
+  </si>
+  <si>
+    <t>rossie.funk@yahoo.com</t>
+  </si>
+  <si>
+    <t>armstrong.dangelo@hotmail.com</t>
+  </si>
+  <si>
+    <t>tjacobi@pagac.net</t>
+  </si>
+  <si>
+    <t>marvin.valentin@wiza.com</t>
+  </si>
+  <si>
+    <t>jkozey@zboncak.com</t>
+  </si>
+  <si>
+    <t>schaden.myles@yahoo.com</t>
+  </si>
+  <si>
+    <t>darrell.ohara@kunde.com</t>
+  </si>
+  <si>
+    <t>mcglynn.noemie@yahoo.com</t>
+  </si>
+  <si>
+    <t>white.retta@miller.com</t>
+  </si>
+  <si>
+    <t>vivian.monahan@yahoo.com</t>
+  </si>
+  <si>
+    <t>zackery55@yahoo.com</t>
+  </si>
+  <si>
+    <t>tessie95@abernathy.com</t>
+  </si>
+  <si>
+    <t>christian.mante@gibson.info</t>
+  </si>
+  <si>
+    <t>madelyn30@gleason.com</t>
+  </si>
+  <si>
+    <t>fisher.keely@gmail.com</t>
+  </si>
+  <si>
+    <t>gleason.gaylord@gislason.biz</t>
+  </si>
+  <si>
+    <t>issac30@abernathy.com</t>
+  </si>
+  <si>
+    <t>bconsidine@yahoo.com</t>
+  </si>
+  <si>
+    <t>dubuque.summer@hoeger.org</t>
+  </si>
+  <si>
+    <t>maryse.oberbrunner@yahoo.com</t>
+  </si>
+  <si>
+    <t>gutkowski.isac@mcdermott.com</t>
+  </si>
+  <si>
+    <t>name07@hotmail.com</t>
+  </si>
+  <si>
+    <t>Cornelius</t>
+  </si>
+  <si>
+    <t>Damon</t>
+  </si>
+  <si>
+    <t>Tristian</t>
+  </si>
+  <si>
+    <t>Emelie</t>
+  </si>
+  <si>
+    <t>Kenna</t>
+  </si>
+  <si>
+    <t>Sonny</t>
+  </si>
+  <si>
+    <t>Lilian</t>
+  </si>
+  <si>
+    <t>Paolo</t>
+  </si>
+  <si>
+    <t>Piper</t>
+  </si>
+  <si>
+    <t>Amara</t>
+  </si>
+  <si>
+    <t>Cayla</t>
+  </si>
+  <si>
+    <t>Tre</t>
+  </si>
+  <si>
+    <t>Claud</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Domenic</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Twila</t>
+  </si>
+  <si>
+    <t>Terrill</t>
+  </si>
+  <si>
+    <t>Kolby</t>
+  </si>
+  <si>
+    <t>Darien</t>
+  </si>
+  <si>
+    <t>Beau</t>
+  </si>
+  <si>
+    <t>Marlin</t>
+  </si>
+  <si>
+    <t>Sigmund</t>
+  </si>
+  <si>
+    <t>Isaias</t>
+  </si>
+  <si>
+    <t>Bertram</t>
+  </si>
+  <si>
+    <t>Salvatore</t>
+  </si>
+  <si>
+    <t>Dax</t>
+  </si>
+  <si>
+    <t>Marjory</t>
+  </si>
+  <si>
+    <t>Okey</t>
+  </si>
+  <si>
+    <t>Ericka</t>
+  </si>
+  <si>
+    <t>Sylvia</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Sharon</t>
+  </si>
+  <si>
+    <t>Dora</t>
+  </si>
+  <si>
+    <t>Kris</t>
+  </si>
+  <si>
+    <t>Jaylon</t>
+  </si>
+  <si>
+    <t>Aurelia</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Marcelle</t>
+  </si>
+  <si>
+    <t>Lemuel</t>
+  </si>
+  <si>
+    <t>Zack</t>
+  </si>
+  <si>
+    <t>Winona</t>
+  </si>
+  <si>
+    <t>Libbie</t>
+  </si>
+  <si>
+    <t>Rebeka</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>Hester</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Hobart</t>
+  </si>
+  <si>
+    <t>Ashleigh</t>
+  </si>
+  <si>
+    <t>Elliot</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Elda</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Cheyanne</t>
+  </si>
+  <si>
+    <t>Garnett</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Ephraim</t>
+  </si>
+  <si>
+    <t>Kira</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Jaycee</t>
+  </si>
+  <si>
+    <t>Octavia</t>
+  </si>
+  <si>
+    <t>Reba</t>
+  </si>
+  <si>
+    <t>Grayce</t>
+  </si>
+  <si>
+    <t>Camron</t>
+  </si>
+  <si>
+    <t>Toby</t>
+  </si>
+  <si>
+    <t>Blanca</t>
+  </si>
+  <si>
+    <t>Leif</t>
+  </si>
+  <si>
+    <t>Emilie</t>
+  </si>
+  <si>
+    <t>Amelie</t>
+  </si>
+  <si>
+    <t>Darius</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Heidi</t>
+  </si>
+  <si>
+    <t>Olin</t>
+  </si>
+  <si>
+    <t>Duane</t>
+  </si>
+  <si>
+    <t>Tianna</t>
+  </si>
+  <si>
+    <t>Justen</t>
+  </si>
+  <si>
+    <t>Berta</t>
+  </si>
+  <si>
+    <t>Kristin</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>Nyah</t>
+  </si>
+  <si>
+    <t>Queenie</t>
+  </si>
+  <si>
+    <t>Pattie</t>
+  </si>
+  <si>
+    <t>Lorenza</t>
+  </si>
+  <si>
+    <t>Jadon</t>
+  </si>
+  <si>
+    <t>Rhett</t>
+  </si>
+  <si>
+    <t>Waino</t>
+  </si>
+  <si>
+    <t>Sven</t>
+  </si>
+  <si>
+    <t>Naomi</t>
+  </si>
+  <si>
+    <t>Elaina</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Nathanael</t>
+  </si>
+  <si>
+    <t>Jaylan</t>
+  </si>
+  <si>
+    <t>Zion</t>
+  </si>
+  <si>
+    <t>Deven</t>
+  </si>
+  <si>
+    <t>Emmitt</t>
+  </si>
+  <si>
+    <t>11 Year</t>
+  </si>
+  <si>
+    <t>12 Year</t>
+  </si>
+  <si>
+    <t>13 Year</t>
+  </si>
+  <si>
+    <t>14 Year</t>
+  </si>
+  <si>
+    <t>15 Year</t>
+  </si>
+  <si>
+    <t>16 Year</t>
+  </si>
+  <si>
+    <t>17 Year</t>
+  </si>
+  <si>
+    <t>18 Year</t>
+  </si>
+  <si>
+    <t>19 Year</t>
+  </si>
+  <si>
+    <t>20 Year</t>
+  </si>
+  <si>
+    <t>21 Year</t>
+  </si>
+  <si>
+    <t>22 Year</t>
+  </si>
+  <si>
+    <t>23 Year</t>
+  </si>
+  <si>
+    <t>24 Year</t>
+  </si>
+  <si>
+    <t>25 Year</t>
+  </si>
+  <si>
+    <t>26 Year</t>
+  </si>
+  <si>
+    <t>27 Year</t>
+  </si>
+  <si>
+    <t>28 Year</t>
+  </si>
+  <si>
+    <t>29 Year</t>
+  </si>
+  <si>
+    <t>30 Year</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>5 Year</t>
   </si>
 </sst>
 </file>
@@ -381,12 +985,19 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -455,6 +1066,25 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -475,62 +1105,66 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1246,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1290,22 +1924,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7008955400</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1234567899</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>78</v>
       </c>
       <c r="G2" s="1">
         <v>5</v>
@@ -1314,27 +1948,27 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>83</v>
+        <v>198</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="C3" s="1">
-        <v>7008955489</v>
+        <v>7008955401</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="G3" s="1">
         <v>2.62</v>
@@ -1342,28 +1976,28 @@
       <c r="H3" s="1">
         <v>5.6</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>81</v>
+      <c r="I3" s="22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4">
-        <v>7008957789</v>
+        <v>99</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7008955402</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>89</v>
+      <c r="F4" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="G4" s="1">
         <v>2.62</v>
@@ -1371,28 +2005,28 @@
       <c r="H4" s="1">
         <v>4.5</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>81</v>
+      <c r="I4" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>200</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1">
-        <v>2378654879</v>
+        <v>7008955403</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="G5" s="1">
         <v>2.62</v>
@@ -1400,28 +2034,28 @@
       <c r="H5" s="1">
         <v>6</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>105</v>
+      <c r="I5" s="23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1">
-        <v>2378654880</v>
+        <v>7008955404</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>93</v>
+        <v>75</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="G6" s="1">
         <v>2.62</v>
@@ -1429,28 +2063,28 @@
       <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>106</v>
+      <c r="I6" s="23" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1">
-        <v>2378654881</v>
+        <v>7008955405</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>95</v>
+        <v>75</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="G7" s="1">
         <v>2.62</v>
@@ -1458,28 +2092,28 @@
       <c r="H7" s="1">
         <v>9</v>
       </c>
-      <c r="I7" s="24" t="s">
-        <v>107</v>
+      <c r="I7" s="23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1">
-        <v>2378654882</v>
+        <v>7008955406</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="G8" s="1">
         <v>2.62</v>
@@ -1487,28 +2121,28 @@
       <c r="H8" s="1">
         <v>8.6</v>
       </c>
-      <c r="I8" s="24" t="s">
-        <v>81</v>
+      <c r="I8" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1">
-        <v>2378654883</v>
+        <v>7008955407</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>98</v>
+        <v>75</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="G9" s="1">
         <v>2.62</v>
@@ -1516,28 +2150,28 @@
       <c r="H9" s="1">
         <v>4.2</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>81</v>
+      <c r="I9" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1">
-        <v>2378654884</v>
+        <v>7008955408</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="G10" s="1">
         <v>2.62</v>
@@ -1545,28 +2179,28 @@
       <c r="H10" s="1">
         <v>7.9</v>
       </c>
-      <c r="I10" s="24" t="s">
-        <v>106</v>
+      <c r="I10" s="23" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C11" s="1">
-        <v>2378634884</v>
+        <v>7008955409</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="G11" s="1">
         <v>2.62</v>
@@ -1574,24 +2208,2663 @@
       <c r="H11" s="1">
         <v>7.9</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>106</v>
+      <c r="I11" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7008955410</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="27">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>9</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7008955411</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="27">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7008955412</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="27">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7008955413</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7008955414</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7008955415</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1">
+        <v>9</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7008955416</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7008955417</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19">
+        <v>5.5</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7008955418</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20">
+        <v>5.5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7008955419</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21">
+        <v>5.5</v>
+      </c>
+      <c r="H21" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1">
+        <v>7008955420</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22">
+        <v>5.5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>9</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7008955421</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23">
+        <v>5.5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7008955422</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24">
+        <v>5.5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7008955423</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25">
+        <v>5.5</v>
+      </c>
+      <c r="H25" s="1">
+        <v>6</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7008955424</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>5.5</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="1">
+        <v>7008955425</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27">
+        <v>5.5</v>
+      </c>
+      <c r="H27" s="1">
+        <v>9</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="1">
+        <v>7008955426</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28">
+        <v>5.5</v>
+      </c>
+      <c r="H28" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="1">
+        <v>7008955427</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29">
+        <v>5.5</v>
+      </c>
+      <c r="H29" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>225</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="1">
+        <v>7008955428</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30">
+        <v>5.5</v>
+      </c>
+      <c r="H30" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="1">
+        <v>7008955429</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31">
+        <v>5.5</v>
+      </c>
+      <c r="H31" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="1">
+        <v>7008955430</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32">
+        <v>6.6</v>
+      </c>
+      <c r="H32" s="1">
+        <v>9</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="1">
+        <v>7008955431</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33">
+        <v>6.6</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="1">
+        <v>7008955432</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34">
+        <v>6.6</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="1">
+        <v>7008955433</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35">
+        <v>6.6</v>
+      </c>
+      <c r="H35" s="1">
+        <v>6</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="1">
+        <v>7008955434</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36">
+        <v>6.6</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="1">
+        <v>7008955435</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37">
+        <v>6.6</v>
+      </c>
+      <c r="H37" s="1">
+        <v>9</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="1">
+        <v>7008955436</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38">
+        <v>6.6</v>
+      </c>
+      <c r="H38" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>234</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="1">
+        <v>7008955437</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39">
+        <v>6.6</v>
+      </c>
+      <c r="H39" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="1">
+        <v>7008955438</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40">
+        <v>6.6</v>
+      </c>
+      <c r="H40" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="1">
+        <v>7008955439</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41">
+        <v>6.6</v>
+      </c>
+      <c r="H41" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="1">
+        <v>7008955440</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42">
+        <v>6.6</v>
+      </c>
+      <c r="H42" s="1">
+        <v>9</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>238</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="1">
+        <v>7008955441</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43">
+        <v>6.6</v>
+      </c>
+      <c r="H43" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="1">
+        <v>7008955442</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44">
+        <v>6.6</v>
+      </c>
+      <c r="H44" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="1">
+        <v>7008955443</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45">
+        <v>6.6</v>
+      </c>
+      <c r="H45" s="1">
+        <v>6</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>241</v>
+      </c>
+      <c r="B46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="1">
+        <v>7008955444</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G46">
+        <v>6.6</v>
+      </c>
+      <c r="H46" s="1">
+        <v>4</v>
+      </c>
+      <c r="I46" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="1">
+        <v>7008955445</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G47">
+        <v>6.6</v>
+      </c>
+      <c r="H47" s="1">
+        <v>9</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="1">
+        <v>7008955446</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48">
+        <v>6.6</v>
+      </c>
+      <c r="H48" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>244</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="1">
+        <v>7008955447</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49">
+        <v>6.6</v>
+      </c>
+      <c r="H49" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>245</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="1">
+        <v>7008955448</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G50">
+        <v>6.6</v>
+      </c>
+      <c r="H50" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I50" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>244</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1">
+        <v>7008955449</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51">
+        <v>6.6</v>
+      </c>
+      <c r="H51" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I51" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="1">
+        <v>7008955450</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52">
+        <v>6.6</v>
+      </c>
+      <c r="H52" s="1">
+        <v>9</v>
+      </c>
+      <c r="I52" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="1">
+        <v>7008955451</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53">
+        <v>6.6</v>
+      </c>
+      <c r="H53" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="1">
+        <v>7008955452</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54">
+        <v>6.6</v>
+      </c>
+      <c r="H54" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="1">
+        <v>7008955453</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55">
+        <v>6.6</v>
+      </c>
+      <c r="H55" s="1">
+        <v>6</v>
+      </c>
+      <c r="I55" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>250</v>
+      </c>
+      <c r="B56" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="1">
+        <v>7008955454</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G56">
+        <v>6.6</v>
+      </c>
+      <c r="H56" s="1">
+        <v>4</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="1">
+        <v>7008955455</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G57">
+        <v>6.6</v>
+      </c>
+      <c r="H57" s="1">
+        <v>9</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>252</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="1">
+        <v>7008955456</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58">
+        <v>6.6</v>
+      </c>
+      <c r="H58" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" s="1">
+        <v>7008955457</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G59">
+        <v>6.6</v>
+      </c>
+      <c r="H59" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>254</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" s="1">
+        <v>7008955458</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G60">
+        <v>6.6</v>
+      </c>
+      <c r="H60" s="1">
+        <v>9</v>
+      </c>
+      <c r="I60" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>255</v>
+      </c>
+      <c r="B61" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" s="1">
+        <v>7008955459</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G61">
+        <v>6.6</v>
+      </c>
+      <c r="H61" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>256</v>
+      </c>
+      <c r="B62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="1">
+        <v>7008955460</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G62">
+        <v>6.6</v>
+      </c>
+      <c r="H62" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>257</v>
+      </c>
+      <c r="B63" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="1">
+        <v>7008955461</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63">
+        <v>6.6</v>
+      </c>
+      <c r="H63" s="1">
+        <v>6</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="1">
+        <v>7008955462</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G64">
+        <v>6.6</v>
+      </c>
+      <c r="H64" s="1">
+        <v>4</v>
+      </c>
+      <c r="I64" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>259</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="1">
+        <v>7008955463</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G65">
+        <v>6.6</v>
+      </c>
+      <c r="H65" s="1">
+        <v>9</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>260</v>
+      </c>
+      <c r="B66" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7008955464</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G66">
+        <v>6.6</v>
+      </c>
+      <c r="H66" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I66" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67" t="s">
+        <v>162</v>
+      </c>
+      <c r="C67" s="1">
+        <v>7008955465</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G67">
+        <v>6.6</v>
+      </c>
+      <c r="H67" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>262</v>
+      </c>
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="1">
+        <v>7008955466</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G68">
+        <v>6.6</v>
+      </c>
+      <c r="H68" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="1">
+        <v>7008955467</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G69">
+        <v>6.6</v>
+      </c>
+      <c r="H69" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I69" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>264</v>
+      </c>
+      <c r="B70" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="1">
+        <v>7008955468</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G70">
+        <v>6.6</v>
+      </c>
+      <c r="H70" s="1">
+        <v>9</v>
+      </c>
+      <c r="I70" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>265</v>
+      </c>
+      <c r="B71" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="1">
+        <v>7008955469</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F71" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G71">
+        <v>6.6</v>
+      </c>
+      <c r="H71" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B72" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="1">
+        <v>7008955470</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G72">
+        <v>6.6</v>
+      </c>
+      <c r="H72" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>267</v>
+      </c>
+      <c r="B73" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="1">
+        <v>7008955471</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G73">
+        <v>6.6</v>
+      </c>
+      <c r="H73" s="1">
+        <v>6</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>268</v>
+      </c>
+      <c r="B74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" s="1">
+        <v>7008955472</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G74">
+        <v>6.6</v>
+      </c>
+      <c r="H74" s="1">
+        <v>9</v>
+      </c>
+      <c r="I74" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="1">
+        <v>7008955473</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G75">
+        <v>6.6</v>
+      </c>
+      <c r="H75" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7008955474</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F76" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G76">
+        <v>6.6</v>
+      </c>
+      <c r="H76" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>271</v>
+      </c>
+      <c r="B77" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="1">
+        <v>7008955475</v>
+      </c>
+      <c r="D77" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G77">
+        <v>6.6</v>
+      </c>
+      <c r="H77" s="1">
+        <v>6</v>
+      </c>
+      <c r="I77" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" s="1">
+        <v>7008955476</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G78">
+        <v>6.6</v>
+      </c>
+      <c r="H78" s="1">
+        <v>4</v>
+      </c>
+      <c r="I78" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>273</v>
+      </c>
+      <c r="B79" t="s">
+        <v>174</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7008955477</v>
+      </c>
+      <c r="D79" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G79">
+        <v>6.6</v>
+      </c>
+      <c r="H79" s="1">
+        <v>9</v>
+      </c>
+      <c r="I79" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>274</v>
+      </c>
+      <c r="B80" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="1">
+        <v>7008955478</v>
+      </c>
+      <c r="D80" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G80">
+        <v>6.6</v>
+      </c>
+      <c r="H80" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I80" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>275</v>
+      </c>
+      <c r="B81" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" s="1">
+        <v>7008955479</v>
+      </c>
+      <c r="D81" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G81">
+        <v>6.6</v>
+      </c>
+      <c r="H81" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I81" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>276</v>
+      </c>
+      <c r="B82" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" s="1">
+        <v>7008955480</v>
+      </c>
+      <c r="D82" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G82">
+        <v>6.6</v>
+      </c>
+      <c r="H82" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I82" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>277</v>
+      </c>
+      <c r="B83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="1">
+        <v>7008955481</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E83" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G83">
+        <v>6.6</v>
+      </c>
+      <c r="H83" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>278</v>
+      </c>
+      <c r="B84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" s="1">
+        <v>7008955482</v>
+      </c>
+      <c r="D84" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G84">
+        <v>6.6</v>
+      </c>
+      <c r="H84" s="1">
+        <v>9</v>
+      </c>
+      <c r="I84" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>279</v>
+      </c>
+      <c r="B85" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" s="1">
+        <v>7008955483</v>
+      </c>
+      <c r="D85" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G85">
+        <v>6.6</v>
+      </c>
+      <c r="H85" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I85" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>280</v>
+      </c>
+      <c r="B86" t="s">
+        <v>181</v>
+      </c>
+      <c r="C86" s="1">
+        <v>7008955484</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E86" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F86" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G86">
+        <v>6.6</v>
+      </c>
+      <c r="H86" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I86" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>281</v>
+      </c>
+      <c r="B87" t="s">
+        <v>182</v>
+      </c>
+      <c r="C87" s="1">
+        <v>7008955485</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="F87" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G87">
+        <v>6.6</v>
+      </c>
+      <c r="H87" s="1">
+        <v>6</v>
+      </c>
+      <c r="I87" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>282</v>
+      </c>
+      <c r="B88" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" s="1">
+        <v>7008955486</v>
+      </c>
+      <c r="D88" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E88" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="F88" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G88">
+        <v>6.6</v>
+      </c>
+      <c r="H88" s="1">
+        <v>4</v>
+      </c>
+      <c r="I88" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>283</v>
+      </c>
+      <c r="B89" t="s">
+        <v>184</v>
+      </c>
+      <c r="C89" s="1">
+        <v>7008955487</v>
+      </c>
+      <c r="D89" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F89" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G89">
+        <v>6.6</v>
+      </c>
+      <c r="H89" s="1">
+        <v>9</v>
+      </c>
+      <c r="I89" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" s="1">
+        <v>7008955488</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E90" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="F90" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G90">
+        <v>6.6</v>
+      </c>
+      <c r="H90" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I90" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" t="s">
+        <v>285</v>
+      </c>
+      <c r="B91" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" s="1">
+        <v>7008955489</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="F91" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G91">
+        <v>6.6</v>
+      </c>
+      <c r="H91" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I91" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
+        <v>286</v>
+      </c>
+      <c r="B92" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" s="1">
+        <v>7008955490</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E92" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="F92" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G92">
+        <v>6.6</v>
+      </c>
+      <c r="H92" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I92" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>287</v>
+      </c>
+      <c r="B93" t="s">
+        <v>188</v>
+      </c>
+      <c r="C93" s="1">
+        <v>7008955491</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F93" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G93">
+        <v>6.6</v>
+      </c>
+      <c r="H93" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="I93" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" t="s">
+        <v>288</v>
+      </c>
+      <c r="B94" t="s">
+        <v>189</v>
+      </c>
+      <c r="C94" s="1">
+        <v>7008955492</v>
+      </c>
+      <c r="D94" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F94" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G94">
+        <v>5.5</v>
+      </c>
+      <c r="H94" s="1">
+        <v>9</v>
+      </c>
+      <c r="I94" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" t="s">
+        <v>289</v>
+      </c>
+      <c r="B95" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="1">
+        <v>7008955493</v>
+      </c>
+      <c r="D95" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="F95" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G95">
+        <v>5.5</v>
+      </c>
+      <c r="H95" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I95" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>290</v>
+      </c>
+      <c r="B96" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" s="1">
+        <v>7008955494</v>
+      </c>
+      <c r="D96" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F96" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G96">
+        <v>5.5</v>
+      </c>
+      <c r="H96" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I96" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>291</v>
+      </c>
+      <c r="B97" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="1">
+        <v>7008955495</v>
+      </c>
+      <c r="D97" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F97" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G97">
+        <v>5.5</v>
+      </c>
+      <c r="H97" s="1">
+        <v>6</v>
+      </c>
+      <c r="I97" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>292</v>
+      </c>
+      <c r="B98" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="1">
+        <v>7008955496</v>
+      </c>
+      <c r="D98" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F98" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G98">
+        <v>5.5</v>
+      </c>
+      <c r="H98" s="1">
+        <v>4</v>
+      </c>
+      <c r="I98" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>293</v>
+      </c>
+      <c r="B99" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" s="1">
+        <v>7008955497</v>
+      </c>
+      <c r="D99" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E99" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G99">
+        <v>5.5</v>
+      </c>
+      <c r="H99" s="1">
+        <v>9</v>
+      </c>
+      <c r="I99" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>294</v>
+      </c>
+      <c r="B100" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="1">
+        <v>7008955498</v>
+      </c>
+      <c r="D100" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E100" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F100" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G100">
+        <v>5.5</v>
+      </c>
+      <c r="H100" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="I100" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>295</v>
+      </c>
+      <c r="B101" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="1">
+        <v>7008955499</v>
+      </c>
+      <c r="D101" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F101" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G101">
+        <v>5.5</v>
+      </c>
+      <c r="H101" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="I101" s="23" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75">
+      <c r="A2" s="29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75">
+      <c r="A3" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75">
+      <c r="A5" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>